<commit_message>
survival calculations from field data
</commit_message>
<xml_diff>
--- a/inst/extdata/survival_from_genotype_livedead.xlsx
+++ b/inst/extdata/survival_from_genotype_livedead.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="10584"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23016" windowHeight="10584"/>
   </bookViews>
   <sheets>
     <sheet name="kolaczinski2000_kdr_survival" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Etofenprox</t>
   </si>
@@ -89,15 +89,6 @@
     <t>Study</t>
   </si>
   <si>
-    <t>Kolaczinski2001</t>
-  </si>
-  <si>
-    <t>Kolaczinski2002</t>
-  </si>
-  <si>
-    <t>Kolaczinski2003</t>
-  </si>
-  <si>
     <t>species</t>
   </si>
   <si>
@@ -140,19 +131,22 @@
     <t>Essandoh2013 A</t>
   </si>
   <si>
-    <t>Essandoh2014 B</t>
-  </si>
-  <si>
-    <t>Essandoh2015 C</t>
-  </si>
-  <si>
-    <t>Essandoh2016 D</t>
-  </si>
-  <si>
     <t>no live or dead ss</t>
   </si>
   <si>
     <t>freq R</t>
+  </si>
+  <si>
+    <t>seesm not to have control mortality ?</t>
+  </si>
+  <si>
+    <t>Essandoh2013 B</t>
+  </si>
+  <si>
+    <t>Essandoh2013 C</t>
+  </si>
+  <si>
+    <t>Essandoh2013 D</t>
   </si>
 </sst>
 </file>
@@ -168,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +181,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -200,13 +200,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,13 +511,13 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -555,147 +559,147 @@
         <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="9">
         <v>200</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="9">
         <v>92</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="9">
         <v>13</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="9">
         <v>4</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="9">
         <v>17</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="9">
         <v>7</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="9">
         <v>3</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="9">
         <f>F2+I2</f>
         <v>109</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="9">
         <f t="shared" ref="M2:N5" si="0">G2+J2</f>
         <v>20</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="9">
         <f>F2/L2</f>
         <v>0.84403669724770647</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="9">
         <f t="shared" ref="P2:Q5" si="1">G2/M2</f>
         <v>0.65</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="9">
         <f t="shared" si="1"/>
         <v>0.5714285714285714</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="9">
         <f>(L2*2+M2)/(2*(L2+M2+N2))</f>
         <v>0.875</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3">
         <v>20</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>245</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>28</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>10</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>49</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>11</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>7</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <f t="shared" ref="L3:L5" si="2">F3+I3</f>
         <v>294</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="3">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="3">
         <f t="shared" ref="O3:O5" si="3">F3/L3</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="3">
         <f t="shared" si="1"/>
         <v>0.71794871794871795</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="3">
         <f t="shared" si="1"/>
         <v>0.58823529411764708</v>
       </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R9" si="4">(L3*2+M3)/(2*(L3+M3+N3))</f>
+      <c r="R3" s="3">
+        <f t="shared" ref="R3:R10" si="4">(L3*2+M3)/(2*(L3+M3+N3))</f>
         <v>0.89571428571428569</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4">
         <v>200</v>
@@ -747,104 +751,104 @@
         <v>0.84375</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7">
         <v>105</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>17</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="7">
         <v>10</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="7">
         <v>52</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="7">
         <v>17</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="7">
         <v>2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="7">
         <f t="shared" si="2"/>
         <v>157</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="7">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="7">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="7">
         <f t="shared" si="3"/>
         <v>0.66878980891719741</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="7">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="7">
         <f t="shared" si="1"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="7">
         <f t="shared" si="4"/>
         <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="S6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7" s="5">
         <v>16</v>
@@ -865,27 +869,27 @@
         <v>166</v>
       </c>
       <c r="L7" s="5">
-        <f t="shared" ref="L7:L8" si="5">F7+I7</f>
+        <f t="shared" ref="L7:L9" si="5">F7+I7</f>
         <v>19</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" ref="M7:M8" si="6">G7+J7</f>
+        <f t="shared" ref="M7:M9" si="6">G7+J7</f>
         <v>82</v>
       </c>
       <c r="N7" s="5">
-        <f t="shared" ref="N7:N8" si="7">H7+K7</f>
+        <f t="shared" ref="N7:N9" si="7">H7+K7</f>
         <v>169</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" ref="O7:O8" si="8">F7/L7</f>
+        <f t="shared" ref="O7:O9" si="8">F7/L7</f>
         <v>0.84210526315789469</v>
       </c>
       <c r="P7" s="5">
-        <f t="shared" ref="P7:P8" si="9">G7/M7</f>
+        <f t="shared" ref="P7:P9" si="9">G7/M7</f>
         <v>0.56097560975609762</v>
       </c>
       <c r="Q7" s="5">
-        <f t="shared" ref="Q7:Q8" si="10">H7/N7</f>
+        <f t="shared" ref="Q7:Q9" si="10">H7/N7</f>
         <v>1.7751479289940829E-2</v>
       </c>
       <c r="R7" s="5">
@@ -893,144 +897,151 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>8</v>
-      </c>
-      <c r="H8">
-        <v>14</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>12</v>
-      </c>
-      <c r="K8">
-        <v>235</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="7"/>
-        <v>249</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="9"/>
-        <v>0.4</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="10"/>
-        <v>5.6224899598393573E-2</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="4"/>
-        <v>4.0740740740740744E-2</v>
-      </c>
-      <c r="S8" t="s">
-        <v>36</v>
-      </c>
+    <row r="8" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F9">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H9">
+        <v>14</v>
+      </c>
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="I9">
-        <v>4</v>
-      </c>
       <c r="J9">
+        <v>12</v>
+      </c>
+      <c r="K9">
+        <v>235</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="K9">
-        <v>95</v>
-      </c>
-      <c r="L9">
-        <f t="shared" ref="L9" si="11">F9+I9</f>
-        <v>19</v>
-      </c>
-      <c r="M9">
-        <f t="shared" ref="M9" si="12">G9+J9</f>
-        <v>36</v>
-      </c>
       <c r="N9">
-        <f t="shared" ref="N9" si="13">H9+K9</f>
-        <v>95</v>
+        <f t="shared" si="7"/>
+        <v>249</v>
       </c>
       <c r="O9">
-        <f t="shared" ref="O9" si="14">F9/L9</f>
-        <v>0.78947368421052633</v>
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
       <c r="P9">
-        <f t="shared" ref="P9" si="15">G9/M9</f>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="9"/>
+        <v>0.4</v>
       </c>
       <c r="Q9">
-        <f t="shared" ref="Q9" si="16">H9/N9</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>5.6224899598393573E-2</v>
       </c>
       <c r="R9">
         <f t="shared" si="4"/>
-        <v>0.24666666666666667</v>
+        <v>4.0740740740740744E-2</v>
+      </c>
+      <c r="S9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>20</v>
+      </c>
+      <c r="K10">
+        <v>95</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10" si="11">F10+I10</f>
+        <v>19</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="12">G10+J10</f>
+        <v>36</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ref="N10" si="13">H10+K10</f>
+        <v>95</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ref="O10" si="14">F10/L10</f>
+        <v>0.78947368421052633</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ref="P10" si="15">G10/M10</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ref="Q10" si="16">H10/N10</f>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="4"/>
+        <v>0.24666666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>